<commit_message>
use interop excel instead Epplus for report
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTTNM.xlsx
+++ b/ATV_Allowance/Templates/TemplateTTNM.xlsx
@@ -62,9 +62,6 @@
     <t>Cộng</t>
   </si>
   <si>
-    <t>(Thành tiền bằng chữ: Bốn triệu năm trăm năm mươi chín ngàn một trăm đồng)</t>
-  </si>
-  <si>
     <t>Long Xuyên, Ngày 24 tháng 1 năm 2019</t>
   </si>
   <si>
@@ -83,34 +80,6 @@
     <t>THÁNG 12/2018</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">BẢNG TỔNG HỢP NHUẬN BÚT PHÁT THANH </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TRỰC TIẾP</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> (CTV) </t>
   </si>
   <si>
@@ -130,6 +99,12 @@
   </si>
   <si>
     <t>Trừ chỉ tiêu</t>
+  </si>
+  <si>
+    <t>(Thành tiền bằng chữ: Không đồng)</t>
+  </si>
+  <si>
+    <t>BẢNG THÙ LAO TIN, PS TRONG THÔNG TIN NGÀY MỚI</t>
   </si>
 </sst>
 </file>
@@ -140,7 +115,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,15 +154,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -324,6 +290,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -335,30 +325,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,7 +613,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:S5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,84 +653,84 @@
       <c r="T1" s="19"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="A2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M2" s="11"/>
       <c r="N2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="11"/>
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
+      <c r="K3" s="20"/>
+      <c r="L3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18" t="s">
+      <c r="M3" s="20"/>
+      <c r="N3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18" t="s">
+      <c r="O3" s="20"/>
+      <c r="P3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
@@ -801,40 +767,40 @@
       <c r="O4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="18"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="20"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="21"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="14"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -850,7 +816,9 @@
       <c r="P6" s="12"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="6"/>
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D7"/>
@@ -868,7 +836,7 @@
       <c r="P7"/>
       <c r="S7"/>
       <c r="T7" s="7" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -887,16 +855,16 @@
       <c r="P8"/>
       <c r="S8"/>
       <c r="T8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -905,7 +873,7 @@
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
@@ -913,14 +881,11 @@
       <c r="P9"/>
       <c r="S9"/>
       <c r="T9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A2:K2"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="A1:T1"/>
@@ -935,6 +900,9 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>